<commit_message>
Updated spreadsheet for one table, Updated sample gatherer function, need to break up checking into own fucntions. Commentend out or removed old handlers and generators.
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">Sample Set data</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">A# ug/mL</t>
   </si>
   <si>
-    <t xml:space="preserve">Other peak(s) Give as comma sperated values of conc</t>
+    <t xml:space="preserve">Other Peak(s) [Give a list of comma seperated list of rts and conc values, Example: ((2.11, 0.13), (3.25, 0.25))</t>
   </si>
   <si>
     <t xml:space="preserve">100041567 LC80277</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Pass</t>
   </si>
   <si>
-    <t xml:space="preserve">6.23, 2.15, 0.015, 8.23</t>
+    <t xml:space="preserve">(2.11, 0.13), (3.25, 0.25)</t>
   </si>
   <si>
     <t xml:space="preserve">blank</t>
@@ -70,10 +70,16 @@
     <t xml:space="preserve">pass</t>
   </si>
   <si>
+    <t xml:space="preserve">(3.46, 2.99)</t>
+  </si>
+  <si>
     <t xml:space="preserve">sample  </t>
   </si>
   <si>
     <t xml:space="preserve">fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string to fail here</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -381,7 +387,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="63.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="106.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="52.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="63.57"/>
   </cols>
@@ -463,7 +469,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,7 +477,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -480,19 +486,21 @@
         <v>2.12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -501,23 +509,23 @@
         <v>0.82</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0.024</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>7.18</v>
-      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D7" s="2" t="n">
         <v>20.11</v>
       </c>
@@ -527,18 +535,18 @@
       <c r="F7" s="2" t="n">
         <v>0.35</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>500</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D8" s="2" t="n">
         <v>20.22</v>
       </c>
@@ -548,9 +556,7 @@
       <c r="F8" s="3" t="n">
         <v>0.14</v>
       </c>
-      <c r="G8" s="3" t="n">
-        <v>20</v>
-      </c>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -587,83 +593,6 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="F14" s="0"/>
-      <c r="G14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="F17" s="0"/>
-      <c r="G17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="F20" s="0"/>
-      <c r="G20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="F22" s="0"/>
-      <c r="G22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="F23" s="0"/>
-      <c r="G23" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Set sample list checker function, seps inputs for other peaks properly into another list of dicts with retention time and concentration key-value pairs with there numerical values
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t xml:space="preserve">Sample Set data</t>
   </si>
@@ -77,17 +77,15 @@
   </si>
   <si>
     <t xml:space="preserve">fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string to fail here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -169,7 +167,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,6 +177,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,7 +384,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -427,7 +433,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -450,7 +456,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -473,7 +479,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -491,12 +497,10 @@
       <c r="F5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -517,12 +521,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="n">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
@@ -538,7 +540,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -550,49 +552,49 @@
       <c r="D8" s="2" t="n">
         <v>20.22</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="5" t="n">
         <v>0.14</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Todo message so I know where I left off at
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t xml:space="preserve">Sample Set data</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(words, that), (should, fail)</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -497,7 +500,9 @@
       <c r="F5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">

</xml_diff>

<commit_message>
Fixed non-numericals in the list format not causing a sys.exit()
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETZJWX\Documents\CS50P-Work-Folder-\project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F804F0A-E386-4F61-BA41-761E8BCB5F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="3900" yWindow="2670" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -22,102 +27,81 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
-    <t xml:space="preserve">Sample Set data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">units (ug/ml or ug/100cm2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limit (APQL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appearance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A# ug/mL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Peak(s) [Give a list of comma seperated list of rts and conc values, Example: ((2.11, 0.13), (3.25, 0.25))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100041567 LC80277</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ug/ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2.11, 0.13), (3.25, 0.25)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ug/100cm2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3.46, 2.99)</t>
+    <t>Sample Set data</t>
+  </si>
+  <si>
+    <t>Sample ID</t>
+  </si>
+  <si>
+    <t>Sample Type</t>
+  </si>
+  <si>
+    <t>units (ug/ml or ug/100cm2)</t>
+  </si>
+  <si>
+    <t>Limit (APQL)</t>
+  </si>
+  <si>
+    <t>Appearance</t>
+  </si>
+  <si>
+    <t>A# ug/mL</t>
+  </si>
+  <si>
+    <t>Other Peak(s) [Give a list of comma seperated list of rts and conc values, Example: ((2.11, 0.13), (3.25, 0.25))</t>
+  </si>
+  <si>
+    <t>100041567 LC80277</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>ug/ml</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>(2.11, 0.13), (3.25, 0.25)</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>ug/100cm2</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>(3.46, 2.99)</t>
   </si>
   <si>
     <t xml:space="preserve">sample  </t>
   </si>
   <si>
-    <t xml:space="preserve">fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(words, that), (should, fail)</t>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>(This, is not correct), (Nor, is this)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -130,134 +114,107 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285f4"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ea4335"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="fbbc04"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34a853"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="ff6d01"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46bdc6"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -287,7 +244,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -311,7 +268,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -371,48 +328,47 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="106.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="52.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="63.57"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="107" customWidth="1"/>
+    <col min="8" max="8" width="52.42578125" customWidth="1"/>
+    <col min="9" max="10" width="63.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -435,7 +391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -445,21 +401,21 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>1.11</v>
+      <c r="D3" s="2">
+        <v>1.1100000000000001</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -468,21 +424,21 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="2">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -491,21 +447,21 @@
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2">
         <v>2.12</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="2">
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -514,38 +470,38 @@
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="2">
         <v>0.82</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>0.024</v>
+      <c r="F6" s="2">
+        <v>2.4E-2</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+    <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="2">
         <v>20.11</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="2">
         <v>0.35</v>
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+    <row r="8" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -554,18 +510,18 @@
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="2">
         <v>20.22</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <v>0.14</v>
+      <c r="F8" s="5">
+        <v>0.14000000000000001</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -574,7 +530,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -583,7 +539,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -592,7 +548,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -605,12 +561,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added error handling for not linking a file or adding more than one file link
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETZJWX\Documents\CS50P-Work-Folder-\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F804F0A-E386-4F61-BA41-761E8BCB5F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F750013-79DF-4F89-A7B6-BFEB9F07F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2670" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Sample Set data</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>fail</t>
-  </si>
-  <si>
-    <t>(This, is not correct), (Nor, is this)</t>
   </si>
 </sst>
 </file>
@@ -143,10 +140,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,204 +355,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>34</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>10</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>2.12</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0.82</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>20.11</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0.35</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>20.22</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added handler function in statement_gen_lib that directs sample set to build each line of the statment from an empty string var and returns that string after it loops over the entire sample set
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETZJWX\Documents\CS50P-Work-Folder-\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F750013-79DF-4F89-A7B6-BFEB9F07F312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C254E1-EB5B-405C-8209-1D9620C87269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2670" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Sample Set data</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>sample</t>
   </si>
 </sst>
 </file>
@@ -339,8 +342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -480,7 +483,9 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Got program to print sample info and AR for that sample.
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,7 +475,7 @@
         <v>2.12</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0</v>
+        <v>20.222</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Added appearance line gen, and finished and downsized total state gen. Need to code tests
</commit_message>
<xml_diff>
--- a/project/Cleaning Samples Template.xlsx
+++ b/project/Cleaning Samples Template.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">fail</t>
   </si>
   <si>
-    <t xml:space="preserve">sample</t>
+    <t xml:space="preserve">sample </t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>